<commit_message>
Fixed calculation errors on the spreadsheet
Cost went down by a factor of 30 because I used the wrong number somewhere
</commit_message>
<xml_diff>
--- a/Costing.xlsx
+++ b/Costing.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\caleb\OneDrive\Documents\Oxford Future Impact Group\monitoring-amr\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{856145B0-01D3-435F-9591-81A59025BD80}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3D8AF0F-9BE1-48EB-BCF7-4C851A79E778}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{5C58E0DF-9FDC-48B7-923D-8A6BE352DF26}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="42">
   <si>
     <t>gpt-3.5-turbo-0125</t>
   </si>
@@ -119,9 +119,6 @@
     <t>Output Length</t>
   </si>
   <si>
-    <t>Monthly Cost</t>
-  </si>
-  <si>
     <t>Safety Factor</t>
   </si>
   <si>
@@ -149,22 +146,35 @@
     <t>This normalises output.</t>
   </si>
   <si>
-    <t>&lt; $30 a month to analyse 5 articles / day</t>
-  </si>
-  <si>
     <t>Articles / Day</t>
+  </si>
+  <si>
+    <t>Cost / Article</t>
+  </si>
+  <si>
+    <t>Days / Month Active</t>
+  </si>
+  <si>
+    <t>Cost / Day</t>
+  </si>
+  <si>
+    <t>Cost / Month</t>
+  </si>
+  <si>
+    <t>Dollars to pounds</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="5">
+  <numFmts count="6">
     <numFmt numFmtId="44" formatCode="_-&quot;R&quot;* #,##0.00_-;\-&quot;R&quot;* #,##0.00_-;_-&quot;R&quot;* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="168" formatCode="_-[$$-409]* #,##0.00_ ;_-[$$-409]* \-#,##0.00\ ;_-[$$-409]* &quot;-&quot;??_ ;_-@_ "/>
-    <numFmt numFmtId="170" formatCode="_-[$$-409]* #,##0.0000_ ;_-[$$-409]* \-#,##0.0000\ ;_-[$$-409]* &quot;-&quot;??_ ;_-@_ "/>
-    <numFmt numFmtId="171" formatCode="_-[$$-409]* #,##0.00000_ ;_-[$$-409]* \-#,##0.00000\ ;_-[$$-409]* &quot;-&quot;??_ ;_-@_ "/>
-    <numFmt numFmtId="179" formatCode="_-[$$-409]* #,##0.0000_ ;_-[$$-409]* \-#,##0.0000\ ;_-[$$-409]* &quot;-&quot;????_ ;_-@_ "/>
+    <numFmt numFmtId="164" formatCode="_-[$$-409]* #,##0.00_ ;_-[$$-409]* \-#,##0.00\ ;_-[$$-409]* &quot;-&quot;??_ ;_-@_ "/>
+    <numFmt numFmtId="165" formatCode="_-[$$-409]* #,##0.0000_ ;_-[$$-409]* \-#,##0.0000\ ;_-[$$-409]* &quot;-&quot;??_ ;_-@_ "/>
+    <numFmt numFmtId="166" formatCode="_-[$$-409]* #,##0.00000_ ;_-[$$-409]* \-#,##0.00000\ ;_-[$$-409]* &quot;-&quot;??_ ;_-@_ "/>
+    <numFmt numFmtId="167" formatCode="_-[$$-409]* #,##0.0000_ ;_-[$$-409]* \-#,##0.0000\ ;_-[$$-409]* &quot;-&quot;????_ ;_-@_ "/>
+    <numFmt numFmtId="171" formatCode="_-* #,##0.0000\ [$€-1]_-;\-* #,##0.0000\ [$€-1]_-;_-* &quot;-&quot;??\ [$€-1]_-;_-@_-"/>
   </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
@@ -198,21 +208,15 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="0" tint="-4.9989318521683403E-2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="5">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -248,43 +252,13 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -299,21 +273,15 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="171" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
@@ -322,28 +290,28 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="170" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="179" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="171" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -3291,10 +3259,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AC8FEBA5-2290-4CD7-BFD3-660AEDC50028}">
-  <dimension ref="B2:T30"/>
+  <dimension ref="B2:T36"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="66" workbookViewId="0">
-      <selection activeCell="K25" sqref="K25"/>
+    <sheetView tabSelected="1" topLeftCell="D18" zoomScale="128" workbookViewId="0">
+      <selection activeCell="L24" sqref="L24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3302,15 +3270,17 @@
     <col min="1" max="1" width="8.88671875" style="4"/>
     <col min="2" max="2" width="5.44140625" style="4" customWidth="1"/>
     <col min="3" max="3" width="16.77734375" style="4" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.33203125" style="4" customWidth="1"/>
+    <col min="4" max="4" width="8.77734375" style="4" customWidth="1"/>
     <col min="5" max="5" width="8.5546875" style="4" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="9.5546875" style="4" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.88671875" style="4" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.5546875" style="4" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.5546875" style="4" customWidth="1"/>
+    <col min="8" max="8" width="10" style="4" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="9.5546875" style="4" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="9.88671875" style="4" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="14.109375" style="4" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10" style="4" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="16.6640625" style="4" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="16.77734375" style="4" bestFit="1" customWidth="1"/>
-    <col min="13" max="15" width="8.77734375" style="4" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="9.21875" style="4" bestFit="1" customWidth="1"/>
+    <col min="14" max="15" width="8.77734375" style="4" bestFit="1" customWidth="1"/>
     <col min="16" max="18" width="9.88671875" style="4" bestFit="1" customWidth="1"/>
     <col min="19" max="16384" width="8.88671875" style="4"/>
   </cols>
@@ -3319,105 +3289,105 @@
       <c r="B2" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="D2" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="E2" s="5"/>
+      <c r="E2" s="17"/>
       <c r="G2" s="4" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="3" spans="2:20" x14ac:dyDescent="0.3">
-      <c r="C3" s="6" t="s">
+      <c r="C3" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="D3" s="7" t="s">
+      <c r="D3" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="E3" s="7" t="s">
+      <c r="E3" s="6" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="4" spans="2:20" x14ac:dyDescent="0.3">
-      <c r="B4" s="8" t="s">
+      <c r="B4" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="C4" s="6" t="s">
+      <c r="C4" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="D4" s="9">
+      <c r="D4" s="7">
         <v>0.5</v>
       </c>
-      <c r="E4" s="9">
+      <c r="E4" s="7">
         <v>1.5</v>
       </c>
-      <c r="F4" s="5" t="s">
+      <c r="F4" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="G4" s="5"/>
-      <c r="H4" s="5"/>
-      <c r="I4" s="5"/>
-      <c r="J4" s="5"/>
+      <c r="G4" s="17"/>
+      <c r="H4" s="17"/>
+      <c r="I4" s="17"/>
+      <c r="J4" s="17"/>
     </row>
     <row r="5" spans="2:20" x14ac:dyDescent="0.3">
-      <c r="B5" s="8"/>
-      <c r="C5" s="6" t="s">
+      <c r="B5" s="15"/>
+      <c r="C5" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="D5" s="9">
+      <c r="D5" s="7">
         <v>30</v>
       </c>
-      <c r="E5" s="9">
+      <c r="E5" s="7">
         <v>60</v>
       </c>
-      <c r="F5" s="6" t="s">
+      <c r="F5" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="G5" s="6" t="s">
+      <c r="G5" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="H5" s="6" t="s">
+      <c r="H5" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="I5" s="6" t="s">
+      <c r="I5" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="J5" s="6" t="s">
+      <c r="J5" s="5" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="6" spans="2:20" x14ac:dyDescent="0.3">
-      <c r="B6" s="8"/>
-      <c r="C6" s="6" t="s">
+      <c r="B6" s="15"/>
+      <c r="C6" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="D6" s="9">
+      <c r="D6" s="7">
         <v>10</v>
       </c>
-      <c r="E6" s="9">
+      <c r="E6" s="7">
         <v>30</v>
       </c>
-      <c r="F6" s="10">
+      <c r="F6" s="8">
         <v>2.5500000000000002E-3</v>
       </c>
-      <c r="G6" s="10">
+      <c r="G6" s="8">
         <v>7.6499999999999997E-3</v>
       </c>
-      <c r="H6" s="10">
+      <c r="H6" s="8">
         <v>7.6499999999999997E-3</v>
       </c>
-      <c r="I6" s="10">
+      <c r="I6" s="8">
         <v>1.1050000000000001E-2</v>
       </c>
-      <c r="J6" s="10">
+      <c r="J6" s="8">
         <v>1.1050000000000001E-2</v>
       </c>
     </row>
     <row r="8" spans="2:20" x14ac:dyDescent="0.3">
-      <c r="C8" s="6" t="s">
+      <c r="C8" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="D8" s="11">
+      <c r="D8" s="9">
         <f>1000/750</f>
         <v>1.3333333333333333</v>
       </c>
@@ -3426,518 +3396,518 @@
       <c r="B10" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="D10" s="5" t="s">
+      <c r="D10" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="E10" s="5"/>
-      <c r="F10" s="5"/>
-      <c r="G10" s="5"/>
-      <c r="H10" s="5"/>
-      <c r="I10" s="5"/>
-      <c r="J10" s="5"/>
+      <c r="E10" s="17"/>
+      <c r="F10" s="17"/>
+      <c r="G10" s="17"/>
+      <c r="H10" s="17"/>
+      <c r="I10" s="17"/>
+      <c r="J10" s="17"/>
     </row>
     <row r="11" spans="2:20" x14ac:dyDescent="0.3">
-      <c r="C11" s="6" t="s">
+      <c r="C11" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="D11" s="6">
+      <c r="D11" s="5">
         <v>800</v>
       </c>
-      <c r="E11" s="6">
+      <c r="E11" s="5">
         <v>1000</v>
       </c>
-      <c r="F11" s="6">
+      <c r="F11" s="5">
         <v>1500</v>
       </c>
-      <c r="G11" s="6">
+      <c r="G11" s="5">
         <v>2000</v>
       </c>
-      <c r="H11" s="6">
+      <c r="H11" s="5">
         <v>2500</v>
       </c>
-      <c r="I11" s="6">
+      <c r="I11" s="5">
         <v>3000</v>
       </c>
-      <c r="J11" s="6">
+      <c r="J11" s="5">
         <v>4000</v>
       </c>
-      <c r="L11" s="12" t="s">
+      <c r="L11" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="M11" s="12">
+      <c r="M11" s="10">
         <v>100</v>
       </c>
-      <c r="N11" s="12" t="s">
+      <c r="N11" s="10" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="12" spans="2:20" x14ac:dyDescent="0.3">
-      <c r="B12" s="8" t="s">
+      <c r="B12" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="C12" s="6" t="s">
+      <c r="C12" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="D12" s="13">
+      <c r="D12" s="11">
         <f>D$11*$D4*$D$8/1000000</f>
         <v>5.3333333333333325E-4</v>
       </c>
-      <c r="E12" s="13">
+      <c r="E12" s="11">
         <f t="shared" ref="E12:J12" si="0">E$11*$D4*$D$8/1000000</f>
         <v>6.6666666666666664E-4</v>
       </c>
-      <c r="F12" s="13">
+      <c r="F12" s="11">
         <f t="shared" si="0"/>
         <v>1E-3</v>
       </c>
-      <c r="G12" s="13">
+      <c r="G12" s="11">
         <f t="shared" si="0"/>
         <v>1.3333333333333333E-3</v>
       </c>
-      <c r="H12" s="13">
+      <c r="H12" s="11">
         <f t="shared" si="0"/>
         <v>1.6666666666666666E-3</v>
       </c>
-      <c r="I12" s="13">
+      <c r="I12" s="11">
         <f t="shared" si="0"/>
         <v>2E-3</v>
       </c>
-      <c r="J12" s="13">
+      <c r="J12" s="11">
         <f t="shared" si="0"/>
         <v>2.6666666666666666E-3</v>
       </c>
-      <c r="L12" s="14">
-        <f>D12*$M$11</f>
+      <c r="L12" s="12">
+        <f t="shared" ref="L12:R14" si="1">D12*$M$11</f>
         <v>5.3333333333333323E-2</v>
       </c>
-      <c r="M12" s="14">
-        <f>E12*$M$11</f>
+      <c r="M12" s="12">
+        <f t="shared" si="1"/>
         <v>6.6666666666666666E-2</v>
       </c>
-      <c r="N12" s="14">
-        <f>F12*$M$11</f>
+      <c r="N12" s="12">
+        <f t="shared" si="1"/>
         <v>0.1</v>
       </c>
-      <c r="O12" s="14">
-        <f>G12*$M$11</f>
+      <c r="O12" s="12">
+        <f t="shared" si="1"/>
         <v>0.13333333333333333</v>
       </c>
-      <c r="P12" s="14">
-        <f>H12*$M$11</f>
+      <c r="P12" s="12">
+        <f t="shared" si="1"/>
         <v>0.16666666666666666</v>
       </c>
-      <c r="Q12" s="14">
-        <f>I12*$M$11</f>
+      <c r="Q12" s="12">
+        <f t="shared" si="1"/>
         <v>0.2</v>
       </c>
-      <c r="R12" s="14">
-        <f>J12*$M$11</f>
+      <c r="R12" s="12">
+        <f t="shared" si="1"/>
         <v>0.26666666666666666</v>
       </c>
-      <c r="S12" s="15"/>
-      <c r="T12" s="15"/>
+      <c r="S12" s="13"/>
+      <c r="T12" s="13"/>
     </row>
     <row r="13" spans="2:20" x14ac:dyDescent="0.3">
-      <c r="B13" s="8"/>
-      <c r="C13" s="6" t="s">
+      <c r="B13" s="15"/>
+      <c r="C13" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="D13" s="13">
-        <f t="shared" ref="D13:J13" si="1">D$11*$D5*$D$8/1000000</f>
+      <c r="D13" s="11">
+        <f t="shared" ref="D13:J13" si="2">D$11*$D5*$D$8/1000000</f>
         <v>3.2000000000000001E-2</v>
       </c>
-      <c r="E13" s="13">
+      <c r="E13" s="11">
+        <f t="shared" si="2"/>
+        <v>0.04</v>
+      </c>
+      <c r="F13" s="11">
+        <f t="shared" si="2"/>
+        <v>0.06</v>
+      </c>
+      <c r="G13" s="11">
+        <f t="shared" si="2"/>
+        <v>0.08</v>
+      </c>
+      <c r="H13" s="11">
+        <f t="shared" si="2"/>
+        <v>0.1</v>
+      </c>
+      <c r="I13" s="11">
+        <f t="shared" si="2"/>
+        <v>0.12</v>
+      </c>
+      <c r="J13" s="11">
+        <f t="shared" si="2"/>
+        <v>0.16</v>
+      </c>
+      <c r="L13" s="12">
         <f t="shared" si="1"/>
-        <v>0.04</v>
-      </c>
-      <c r="F13" s="13">
+        <v>3.2</v>
+      </c>
+      <c r="M13" s="12">
         <f t="shared" si="1"/>
-        <v>0.06</v>
-      </c>
-      <c r="G13" s="13">
+        <v>4</v>
+      </c>
+      <c r="N13" s="12">
         <f t="shared" si="1"/>
-        <v>0.08</v>
-      </c>
-      <c r="H13" s="13">
+        <v>6</v>
+      </c>
+      <c r="O13" s="12">
         <f t="shared" si="1"/>
-        <v>0.1</v>
-      </c>
-      <c r="I13" s="13">
+        <v>8</v>
+      </c>
+      <c r="P13" s="12">
         <f t="shared" si="1"/>
-        <v>0.12</v>
-      </c>
-      <c r="J13" s="13">
+        <v>10</v>
+      </c>
+      <c r="Q13" s="12">
         <f t="shared" si="1"/>
-        <v>0.16</v>
-      </c>
-      <c r="L13" s="14">
-        <f>D13*$M$11</f>
-        <v>3.2</v>
-      </c>
-      <c r="M13" s="14">
-        <f>E13*$M$11</f>
-        <v>4</v>
-      </c>
-      <c r="N13" s="14">
-        <f>F13*$M$11</f>
-        <v>6</v>
-      </c>
-      <c r="O13" s="14">
-        <f>G13*$M$11</f>
-        <v>8</v>
-      </c>
-      <c r="P13" s="14">
-        <f>H13*$M$11</f>
-        <v>10</v>
-      </c>
-      <c r="Q13" s="14">
-        <f>I13*$M$11</f>
         <v>12</v>
       </c>
-      <c r="R13" s="14">
-        <f>J13*$M$11</f>
+      <c r="R13" s="12">
+        <f t="shared" si="1"/>
         <v>16</v>
       </c>
-      <c r="S13" s="15"/>
-      <c r="T13" s="15"/>
+      <c r="S13" s="13"/>
+      <c r="T13" s="13"/>
     </row>
     <row r="14" spans="2:20" x14ac:dyDescent="0.3">
-      <c r="B14" s="8"/>
-      <c r="C14" s="6" t="s">
+      <c r="B14" s="15"/>
+      <c r="C14" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="D14" s="13">
-        <f t="shared" ref="D14:J14" si="2">D$11*$D6*$D$8/1000000</f>
+      <c r="D14" s="11">
+        <f t="shared" ref="D14:J14" si="3">D$11*$D6*$D$8/1000000</f>
         <v>1.0666666666666666E-2</v>
       </c>
-      <c r="E14" s="13">
-        <f t="shared" si="2"/>
+      <c r="E14" s="11">
+        <f t="shared" si="3"/>
         <v>1.3333333333333332E-2</v>
       </c>
-      <c r="F14" s="13">
-        <f t="shared" si="2"/>
+      <c r="F14" s="11">
+        <f t="shared" si="3"/>
         <v>0.02</v>
       </c>
-      <c r="G14" s="13">
-        <f t="shared" si="2"/>
+      <c r="G14" s="11">
+        <f t="shared" si="3"/>
         <v>2.6666666666666665E-2</v>
       </c>
-      <c r="H14" s="13">
-        <f t="shared" si="2"/>
+      <c r="H14" s="11">
+        <f t="shared" si="3"/>
         <v>3.3333333333333326E-2</v>
       </c>
-      <c r="I14" s="13">
-        <f t="shared" si="2"/>
+      <c r="I14" s="11">
+        <f t="shared" si="3"/>
         <v>0.04</v>
       </c>
-      <c r="J14" s="13">
-        <f t="shared" si="2"/>
+      <c r="J14" s="11">
+        <f t="shared" si="3"/>
         <v>5.333333333333333E-2</v>
       </c>
-      <c r="L14" s="14">
-        <f>D14*$M$11</f>
+      <c r="L14" s="12">
+        <f t="shared" si="1"/>
         <v>1.0666666666666667</v>
       </c>
-      <c r="M14" s="14">
-        <f>E14*$M$11</f>
+      <c r="M14" s="12">
+        <f t="shared" si="1"/>
         <v>1.3333333333333333</v>
       </c>
-      <c r="N14" s="14">
-        <f>F14*$M$11</f>
+      <c r="N14" s="12">
+        <f t="shared" si="1"/>
         <v>2</v>
       </c>
-      <c r="O14" s="14">
-        <f>G14*$M$11</f>
+      <c r="O14" s="12">
+        <f t="shared" si="1"/>
         <v>2.6666666666666665</v>
       </c>
-      <c r="P14" s="14">
-        <f>H14*$M$11</f>
+      <c r="P14" s="12">
+        <f t="shared" si="1"/>
         <v>3.3333333333333326</v>
       </c>
-      <c r="Q14" s="14">
-        <f>I14*$M$11</f>
+      <c r="Q14" s="12">
+        <f t="shared" si="1"/>
         <v>4</v>
       </c>
-      <c r="R14" s="14">
-        <f>J14*$M$11</f>
+      <c r="R14" s="12">
+        <f t="shared" si="1"/>
         <v>5.333333333333333</v>
       </c>
-      <c r="S14" s="15"/>
-      <c r="T14" s="15"/>
+      <c r="S14" s="13"/>
+      <c r="T14" s="13"/>
     </row>
     <row r="16" spans="2:20" x14ac:dyDescent="0.3">
       <c r="B16" s="3"/>
-      <c r="D16" s="5" t="s">
+      <c r="D16" s="17" t="s">
         <v>21</v>
       </c>
-      <c r="E16" s="5"/>
-      <c r="F16" s="5"/>
-      <c r="G16" s="5"/>
-      <c r="H16" s="5"/>
-      <c r="I16" s="5"/>
-      <c r="J16" s="5"/>
-      <c r="L16" s="16"/>
+      <c r="E16" s="17"/>
+      <c r="F16" s="17"/>
+      <c r="G16" s="17"/>
+      <c r="H16" s="17"/>
+      <c r="I16" s="17"/>
+      <c r="J16" s="17"/>
+      <c r="L16" s="14"/>
     </row>
     <row r="17" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="C17" s="6" t="s">
+      <c r="C17" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="D17" s="6">
+      <c r="D17" s="5">
         <v>30</v>
       </c>
-      <c r="E17" s="6">
+      <c r="E17" s="5">
         <v>40</v>
       </c>
-      <c r="F17" s="6">
+      <c r="F17" s="5">
         <v>50</v>
       </c>
-      <c r="G17" s="6">
+      <c r="G17" s="5">
         <v>75</v>
       </c>
-      <c r="H17" s="6">
+      <c r="H17" s="5">
         <v>100</v>
       </c>
-      <c r="I17" s="6">
+      <c r="I17" s="5">
         <v>150</v>
       </c>
-      <c r="J17" s="6">
+      <c r="J17" s="5">
         <v>200</v>
       </c>
-      <c r="L17" s="12" t="s">
+      <c r="L17" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="M17" s="12">
+      <c r="M17" s="10">
         <v>100</v>
       </c>
-      <c r="N17" s="12" t="s">
+      <c r="N17" s="10" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="18" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B18" s="8" t="s">
+      <c r="B18" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="C18" s="6" t="s">
+      <c r="C18" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="D18" s="13">
+      <c r="D18" s="11">
         <f>D$17*$E4*$D$8/1000000</f>
         <v>6.0000000000000002E-5</v>
       </c>
-      <c r="E18" s="13">
-        <f t="shared" ref="E18:J18" si="3">E$17*$E4*$D$8/1000000</f>
+      <c r="E18" s="11">
+        <f t="shared" ref="E18:J18" si="4">E$17*$E4*$D$8/1000000</f>
         <v>8.0000000000000007E-5</v>
       </c>
-      <c r="F18" s="13">
-        <f t="shared" si="3"/>
+      <c r="F18" s="11">
+        <f t="shared" si="4"/>
         <v>1E-4</v>
       </c>
-      <c r="G18" s="13">
-        <f t="shared" si="3"/>
+      <c r="G18" s="11">
+        <f t="shared" si="4"/>
         <v>1.4999999999999999E-4</v>
       </c>
-      <c r="H18" s="13">
-        <f t="shared" si="3"/>
+      <c r="H18" s="11">
+        <f t="shared" si="4"/>
         <v>2.0000000000000001E-4</v>
       </c>
-      <c r="I18" s="13">
-        <f t="shared" si="3"/>
+      <c r="I18" s="11">
+        <f t="shared" si="4"/>
         <v>2.9999999999999997E-4</v>
       </c>
-      <c r="J18" s="13">
-        <f t="shared" si="3"/>
+      <c r="J18" s="11">
+        <f t="shared" si="4"/>
         <v>4.0000000000000002E-4</v>
       </c>
-      <c r="L18" s="14">
+      <c r="L18" s="12">
         <f>D18*$M$17</f>
         <v>6.0000000000000001E-3</v>
       </c>
-      <c r="M18" s="14">
-        <f t="shared" ref="M18:R18" si="4">E18*$M$17</f>
+      <c r="M18" s="12">
+        <f t="shared" ref="M18:R18" si="5">E18*$M$17</f>
         <v>8.0000000000000002E-3</v>
       </c>
-      <c r="N18" s="14">
-        <f t="shared" si="4"/>
+      <c r="N18" s="12">
+        <f t="shared" si="5"/>
         <v>0.01</v>
       </c>
-      <c r="O18" s="14">
-        <f t="shared" si="4"/>
+      <c r="O18" s="12">
+        <f t="shared" si="5"/>
         <v>1.4999999999999999E-2</v>
       </c>
-      <c r="P18" s="14">
-        <f t="shared" si="4"/>
+      <c r="P18" s="12">
+        <f t="shared" si="5"/>
         <v>0.02</v>
       </c>
-      <c r="Q18" s="14">
-        <f t="shared" si="4"/>
+      <c r="Q18" s="12">
+        <f t="shared" si="5"/>
         <v>0.03</v>
       </c>
-      <c r="R18" s="14">
-        <f t="shared" si="4"/>
+      <c r="R18" s="12">
+        <f t="shared" si="5"/>
         <v>0.04</v>
       </c>
     </row>
     <row r="19" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B19" s="8"/>
-      <c r="C19" s="6" t="s">
+      <c r="B19" s="15"/>
+      <c r="C19" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="D19" s="13">
-        <f t="shared" ref="D19:J20" si="5">D$17*$E5*$D$8/1000000</f>
+      <c r="D19" s="11">
+        <f t="shared" ref="D19:J20" si="6">D$17*$E5*$D$8/1000000</f>
         <v>2.3999999999999998E-3</v>
       </c>
-      <c r="E19" s="13">
-        <f t="shared" si="5"/>
+      <c r="E19" s="11">
+        <f t="shared" si="6"/>
         <v>3.2000000000000002E-3</v>
       </c>
-      <c r="F19" s="13">
-        <f t="shared" si="5"/>
+      <c r="F19" s="11">
+        <f t="shared" si="6"/>
         <v>4.0000000000000001E-3</v>
       </c>
-      <c r="G19" s="13">
-        <f t="shared" si="5"/>
+      <c r="G19" s="11">
+        <f t="shared" si="6"/>
         <v>6.0000000000000001E-3</v>
       </c>
-      <c r="H19" s="13">
-        <f t="shared" si="5"/>
+      <c r="H19" s="11">
+        <f t="shared" si="6"/>
         <v>8.0000000000000002E-3</v>
       </c>
-      <c r="I19" s="13">
-        <f t="shared" si="5"/>
+      <c r="I19" s="11">
+        <f t="shared" si="6"/>
         <v>1.2E-2</v>
       </c>
-      <c r="J19" s="13">
-        <f t="shared" si="5"/>
+      <c r="J19" s="11">
+        <f t="shared" si="6"/>
         <v>1.6E-2</v>
       </c>
-      <c r="L19" s="14">
-        <f t="shared" ref="L19:L20" si="6">D19*$M$17</f>
+      <c r="L19" s="12">
+        <f t="shared" ref="L19:L20" si="7">D19*$M$17</f>
         <v>0.24</v>
       </c>
-      <c r="M19" s="14">
-        <f t="shared" ref="M19:M20" si="7">E19*$M$17</f>
+      <c r="M19" s="12">
+        <f t="shared" ref="M19:M20" si="8">E19*$M$17</f>
         <v>0.32</v>
       </c>
-      <c r="N19" s="14">
-        <f t="shared" ref="N19:N20" si="8">F19*$M$17</f>
+      <c r="N19" s="12">
+        <f t="shared" ref="N19:N20" si="9">F19*$M$17</f>
         <v>0.4</v>
       </c>
-      <c r="O19" s="14">
-        <f t="shared" ref="O19:O20" si="9">G19*$M$17</f>
+      <c r="O19" s="12">
+        <f t="shared" ref="O19:O20" si="10">G19*$M$17</f>
         <v>0.6</v>
       </c>
-      <c r="P19" s="14">
-        <f t="shared" ref="P19:P20" si="10">H19*$M$17</f>
+      <c r="P19" s="12">
+        <f t="shared" ref="P19:P20" si="11">H19*$M$17</f>
         <v>0.8</v>
       </c>
-      <c r="Q19" s="14">
-        <f t="shared" ref="Q19:Q20" si="11">I19*$M$17</f>
+      <c r="Q19" s="12">
+        <f t="shared" ref="Q19:Q20" si="12">I19*$M$17</f>
         <v>1.2</v>
       </c>
-      <c r="R19" s="14">
-        <f t="shared" ref="R19:R20" si="12">J19*$M$17</f>
+      <c r="R19" s="12">
+        <f t="shared" ref="R19:R20" si="13">J19*$M$17</f>
         <v>1.6</v>
       </c>
     </row>
     <row r="20" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B20" s="8"/>
-      <c r="C20" s="6" t="s">
+      <c r="B20" s="15"/>
+      <c r="C20" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="D20" s="13">
-        <f t="shared" si="5"/>
+      <c r="D20" s="11">
+        <f t="shared" si="6"/>
         <v>1.1999999999999999E-3</v>
       </c>
-      <c r="E20" s="13">
-        <f t="shared" si="5"/>
+      <c r="E20" s="11">
+        <f t="shared" si="6"/>
         <v>1.6000000000000001E-3</v>
       </c>
-      <c r="F20" s="13">
-        <f t="shared" si="5"/>
+      <c r="F20" s="11">
+        <f t="shared" si="6"/>
         <v>2E-3</v>
       </c>
-      <c r="G20" s="13">
-        <f t="shared" si="5"/>
+      <c r="G20" s="11">
+        <f t="shared" si="6"/>
         <v>3.0000000000000001E-3</v>
       </c>
-      <c r="H20" s="13">
-        <f t="shared" si="5"/>
+      <c r="H20" s="11">
+        <f t="shared" si="6"/>
         <v>4.0000000000000001E-3</v>
       </c>
-      <c r="I20" s="13">
-        <f t="shared" si="5"/>
+      <c r="I20" s="11">
+        <f t="shared" si="6"/>
         <v>6.0000000000000001E-3</v>
       </c>
-      <c r="J20" s="13">
-        <f t="shared" si="5"/>
+      <c r="J20" s="11">
+        <f t="shared" si="6"/>
         <v>8.0000000000000002E-3</v>
       </c>
-      <c r="L20" s="14">
-        <f t="shared" si="6"/>
+      <c r="L20" s="12">
+        <f t="shared" si="7"/>
         <v>0.12</v>
       </c>
-      <c r="M20" s="14">
-        <f t="shared" si="7"/>
+      <c r="M20" s="12">
+        <f t="shared" si="8"/>
         <v>0.16</v>
       </c>
-      <c r="N20" s="14">
-        <f t="shared" si="8"/>
+      <c r="N20" s="12">
+        <f t="shared" si="9"/>
         <v>0.2</v>
       </c>
-      <c r="O20" s="14">
-        <f t="shared" si="9"/>
+      <c r="O20" s="12">
+        <f t="shared" si="10"/>
         <v>0.3</v>
       </c>
-      <c r="P20" s="14">
-        <f t="shared" si="10"/>
+      <c r="P20" s="12">
+        <f t="shared" si="11"/>
         <v>0.4</v>
       </c>
-      <c r="Q20" s="14">
-        <f t="shared" si="11"/>
+      <c r="Q20" s="12">
+        <f t="shared" si="12"/>
         <v>0.6</v>
       </c>
-      <c r="R20" s="14">
-        <f t="shared" si="12"/>
+      <c r="R20" s="12">
+        <f t="shared" si="13"/>
         <v>0.8</v>
       </c>
     </row>
     <row r="23" spans="2:18" x14ac:dyDescent="0.3">
       <c r="C23" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="D23" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="D23" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="K23" s="19" t="s">
-        <v>30</v>
-      </c>
-      <c r="L23" s="19"/>
+      <c r="K23" s="16" t="s">
+        <v>29</v>
+      </c>
+      <c r="L23" s="16"/>
     </row>
     <row r="24" spans="2:18" x14ac:dyDescent="0.3">
       <c r="D24" s="4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="K24" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="L24" s="1">
-        <v>5</v>
+        <v>15</v>
       </c>
     </row>
     <row r="25" spans="2:18" x14ac:dyDescent="0.3">
       <c r="D25" s="4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="K25" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="L25" s="1">
-        <v>1500</v>
+        <v>3500</v>
       </c>
     </row>
     <row r="26" spans="2:18" x14ac:dyDescent="0.3">
       <c r="D26" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="K26" s="1" t="s">
         <v>25</v>
@@ -3949,37 +3919,76 @@
     </row>
     <row r="27" spans="2:18" x14ac:dyDescent="0.3">
       <c r="D27" s="4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="K27" s="1" t="s">
         <v>26</v>
       </c>
       <c r="L27" s="1">
-        <v>50</v>
+        <v>100</v>
       </c>
     </row>
     <row r="28" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="D28" s="4" t="s">
-        <v>37</v>
-      </c>
       <c r="K28" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="L28" s="1">
         <v>1.2</v>
       </c>
     </row>
-    <row r="29" spans="2:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="K29" s="20"/>
-      <c r="L29" s="20"/>
+    <row r="29" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="K29" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="L29" s="1">
+        <v>31</v>
+      </c>
     </row>
-    <row r="30" spans="2:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="K30" s="17" t="s">
-        <v>27</v>
-      </c>
-      <c r="L30" s="18">
-        <f>L24*31*L28*(L25*VLOOKUP(L26,C4:E6,2,FALSE)+L25*VLOOKUP(L26,C4:E6,3,FALSE)*L27)*D8/1000000</f>
-        <v>28.085999999999999</v>
+    <row r="31" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="K31" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="L31" s="11">
+        <f>L28*(L25*VLOOKUP(L26,C4:E6,2,FALSE)+VLOOKUP(L26,C4:E6,3,FALSE)*L27)*D8/1000000</f>
+        <v>3.0400000000000002E-3</v>
+      </c>
+      <c r="M31" s="18">
+        <f>L31*$L$36</f>
+        <v>2.4016000000000003E-3</v>
+      </c>
+    </row>
+    <row r="32" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="K32" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="L32" s="12">
+        <f>L31*L24</f>
+        <v>4.5600000000000002E-2</v>
+      </c>
+      <c r="M32" s="18">
+        <f t="shared" ref="M32:M33" si="14">L32*$L$36</f>
+        <v>3.6024E-2</v>
+      </c>
+    </row>
+    <row r="33" spans="11:13" x14ac:dyDescent="0.3">
+      <c r="K33" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="L33" s="12">
+        <f>L32*L29</f>
+        <v>1.4136</v>
+      </c>
+      <c r="M33" s="18">
+        <f t="shared" si="14"/>
+        <v>1.116744</v>
+      </c>
+    </row>
+    <row r="36" spans="11:13" x14ac:dyDescent="0.3">
+      <c r="K36" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="L36" s="4">
+        <v>0.79</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
created api and webscraper files
added some text that was retrieved as a prompt from chatgpt
</commit_message>
<xml_diff>
--- a/Costing.xlsx
+++ b/Costing.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\caleb\OneDrive\Documents\Oxford Future Impact Group\monitoring-amr\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3D8AF0F-9BE1-48EB-BCF7-4C851A79E778}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D95AC035-90D4-4CB3-A521-FE68DCBE6866}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{5C58E0DF-9FDC-48B7-923D-8A6BE352DF26}"/>
   </bookViews>
@@ -174,7 +174,7 @@
     <numFmt numFmtId="165" formatCode="_-[$$-409]* #,##0.0000_ ;_-[$$-409]* \-#,##0.0000\ ;_-[$$-409]* &quot;-&quot;??_ ;_-@_ "/>
     <numFmt numFmtId="166" formatCode="_-[$$-409]* #,##0.00000_ ;_-[$$-409]* \-#,##0.00000\ ;_-[$$-409]* &quot;-&quot;??_ ;_-@_ "/>
     <numFmt numFmtId="167" formatCode="_-[$$-409]* #,##0.0000_ ;_-[$$-409]* \-#,##0.0000\ ;_-[$$-409]* &quot;-&quot;????_ ;_-@_ "/>
-    <numFmt numFmtId="171" formatCode="_-* #,##0.0000\ [$€-1]_-;\-* #,##0.0000\ [$€-1]_-;_-* &quot;-&quot;??\ [$€-1]_-;_-@_-"/>
+    <numFmt numFmtId="168" formatCode="_-* #,##0.0000\ [$€-1]_-;\-* #,##0.0000\ [$€-1]_-;_-* &quot;-&quot;??\ [$€-1]_-;_-@_-"/>
   </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
@@ -302,6 +302,9 @@
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="168" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
@@ -310,9 +313,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="171" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -3261,26 +3261,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AC8FEBA5-2290-4CD7-BFD3-660AEDC50028}">
   <dimension ref="B2:T36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D18" zoomScale="128" workbookViewId="0">
-      <selection activeCell="L24" sqref="L24"/>
+    <sheetView tabSelected="1" topLeftCell="A14" zoomScale="106" workbookViewId="0">
+      <selection activeCell="M29" sqref="M29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="8.88671875" style="4"/>
-    <col min="2" max="2" width="5.44140625" style="4" customWidth="1"/>
+    <col min="1" max="2" width="5.44140625" style="4" customWidth="1"/>
     <col min="3" max="3" width="16.77734375" style="4" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.77734375" style="4" customWidth="1"/>
-    <col min="5" max="5" width="8.5546875" style="4" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.5546875" style="4" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.5546875" style="4" customWidth="1"/>
+    <col min="5" max="5" width="8.77734375" style="4" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.88671875" style="4" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="10.5546875" style="4" customWidth="1"/>
-    <col min="8" max="8" width="10" style="4" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.5546875" style="4" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10" style="4" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.21875" style="4" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.88671875" style="4" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.21875" style="4" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="16.6640625" style="4" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="16.77734375" style="4" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="9.21875" style="4" bestFit="1" customWidth="1"/>
-    <col min="14" max="15" width="8.77734375" style="4" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="10.77734375" style="4" bestFit="1" customWidth="1"/>
+    <col min="14" max="15" width="9.21875" style="4" bestFit="1" customWidth="1"/>
     <col min="16" max="18" width="9.88671875" style="4" bestFit="1" customWidth="1"/>
     <col min="19" max="16384" width="8.88671875" style="4"/>
   </cols>
@@ -3289,10 +3288,10 @@
       <c r="B2" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="17" t="s">
+      <c r="D2" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="E2" s="17"/>
+      <c r="E2" s="18"/>
       <c r="G2" s="4" t="s">
         <v>18</v>
       </c>
@@ -3309,7 +3308,7 @@
       </c>
     </row>
     <row r="4" spans="2:20" x14ac:dyDescent="0.3">
-      <c r="B4" s="15" t="s">
+      <c r="B4" s="16" t="s">
         <v>16</v>
       </c>
       <c r="C4" s="5" t="s">
@@ -3321,16 +3320,16 @@
       <c r="E4" s="7">
         <v>1.5</v>
       </c>
-      <c r="F4" s="17" t="s">
+      <c r="F4" s="18" t="s">
         <v>22</v>
       </c>
-      <c r="G4" s="17"/>
-      <c r="H4" s="17"/>
-      <c r="I4" s="17"/>
-      <c r="J4" s="17"/>
+      <c r="G4" s="18"/>
+      <c r="H4" s="18"/>
+      <c r="I4" s="18"/>
+      <c r="J4" s="18"/>
     </row>
     <row r="5" spans="2:20" x14ac:dyDescent="0.3">
-      <c r="B5" s="15"/>
+      <c r="B5" s="16"/>
       <c r="C5" s="5" t="s">
         <v>3</v>
       </c>
@@ -3357,7 +3356,7 @@
       </c>
     </row>
     <row r="6" spans="2:20" x14ac:dyDescent="0.3">
-      <c r="B6" s="15"/>
+      <c r="B6" s="16"/>
       <c r="C6" s="5" t="s">
         <v>4</v>
       </c>
@@ -3396,15 +3395,15 @@
       <c r="B10" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="D10" s="17" t="s">
+      <c r="D10" s="18" t="s">
         <v>13</v>
       </c>
-      <c r="E10" s="17"/>
-      <c r="F10" s="17"/>
-      <c r="G10" s="17"/>
-      <c r="H10" s="17"/>
-      <c r="I10" s="17"/>
-      <c r="J10" s="17"/>
+      <c r="E10" s="18"/>
+      <c r="F10" s="18"/>
+      <c r="G10" s="18"/>
+      <c r="H10" s="18"/>
+      <c r="I10" s="18"/>
+      <c r="J10" s="18"/>
     </row>
     <row r="11" spans="2:20" x14ac:dyDescent="0.3">
       <c r="C11" s="5" t="s">
@@ -3442,7 +3441,7 @@
       </c>
     </row>
     <row r="12" spans="2:20" x14ac:dyDescent="0.3">
-      <c r="B12" s="15" t="s">
+      <c r="B12" s="16" t="s">
         <v>16</v>
       </c>
       <c r="C12" s="5" t="s">
@@ -3508,7 +3507,7 @@
       <c r="T12" s="13"/>
     </row>
     <row r="13" spans="2:20" x14ac:dyDescent="0.3">
-      <c r="B13" s="15"/>
+      <c r="B13" s="16"/>
       <c r="C13" s="5" t="s">
         <v>3</v>
       </c>
@@ -3572,7 +3571,7 @@
       <c r="T13" s="13"/>
     </row>
     <row r="14" spans="2:20" x14ac:dyDescent="0.3">
-      <c r="B14" s="15"/>
+      <c r="B14" s="16"/>
       <c r="C14" s="5" t="s">
         <v>4</v>
       </c>
@@ -3637,15 +3636,15 @@
     </row>
     <row r="16" spans="2:20" x14ac:dyDescent="0.3">
       <c r="B16" s="3"/>
-      <c r="D16" s="17" t="s">
+      <c r="D16" s="18" t="s">
         <v>21</v>
       </c>
-      <c r="E16" s="17"/>
-      <c r="F16" s="17"/>
-      <c r="G16" s="17"/>
-      <c r="H16" s="17"/>
-      <c r="I16" s="17"/>
-      <c r="J16" s="17"/>
+      <c r="E16" s="18"/>
+      <c r="F16" s="18"/>
+      <c r="G16" s="18"/>
+      <c r="H16" s="18"/>
+      <c r="I16" s="18"/>
+      <c r="J16" s="18"/>
       <c r="L16" s="14"/>
     </row>
     <row r="17" spans="2:18" x14ac:dyDescent="0.3">
@@ -3684,7 +3683,7 @@
       </c>
     </row>
     <row r="18" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B18" s="15" t="s">
+      <c r="B18" s="16" t="s">
         <v>16</v>
       </c>
       <c r="C18" s="5" t="s">
@@ -3748,7 +3747,7 @@
       </c>
     </row>
     <row r="19" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B19" s="15"/>
+      <c r="B19" s="16"/>
       <c r="C19" s="5" t="s">
         <v>3</v>
       </c>
@@ -3810,7 +3809,7 @@
       </c>
     </row>
     <row r="20" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B20" s="15"/>
+      <c r="B20" s="16"/>
       <c r="C20" s="5" t="s">
         <v>4</v>
       </c>
@@ -3878,10 +3877,10 @@
       <c r="D23" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="K23" s="16" t="s">
+      <c r="K23" s="17" t="s">
         <v>29</v>
       </c>
-      <c r="L23" s="16"/>
+      <c r="L23" s="17"/>
     </row>
     <row r="24" spans="2:18" x14ac:dyDescent="0.3">
       <c r="D24" s="4" t="s">
@@ -3952,7 +3951,7 @@
         <f>L28*(L25*VLOOKUP(L26,C4:E6,2,FALSE)+VLOOKUP(L26,C4:E6,3,FALSE)*L27)*D8/1000000</f>
         <v>3.0400000000000002E-3</v>
       </c>
-      <c r="M31" s="18">
+      <c r="M31" s="15">
         <f>L31*$L$36</f>
         <v>2.4016000000000003E-3</v>
       </c>
@@ -3965,7 +3964,7 @@
         <f>L31*L24</f>
         <v>4.5600000000000002E-2</v>
       </c>
-      <c r="M32" s="18">
+      <c r="M32" s="15">
         <f t="shared" ref="M32:M33" si="14">L32*$L$36</f>
         <v>3.6024E-2</v>
       </c>
@@ -3978,16 +3977,16 @@
         <f>L32*L29</f>
         <v>1.4136</v>
       </c>
-      <c r="M33" s="18">
+      <c r="M33" s="15">
         <f t="shared" si="14"/>
         <v>1.116744</v>
       </c>
     </row>
     <row r="36" spans="11:13" x14ac:dyDescent="0.3">
-      <c r="K36" s="4" t="s">
+      <c r="K36" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="L36" s="4">
+      <c r="L36" s="1">
         <v>0.79</v>
       </c>
     </row>

</xml_diff>